<commit_message>
nano timer for tones, parse TONE string.
</commit_message>
<xml_diff>
--- a/src/main/resources/devices/Referees.xlsx
+++ b/src/main/resources/devices/Referees.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\owlcms-firmata\src\main\resources\devices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F30572-412D-4D21-A9F6-F24A869BEFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE0ABF4-1D39-4677-9540-B0B494745665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3615" yWindow="2070" windowWidth="21600" windowHeight="11295" xr2:uid="{F9C8F068-60C0-4FDD-8C1E-880F519290ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F9C8F068-60C0-4FDD-8C1E-880F519290ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Referee" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="56">
   <si>
     <t>pin</t>
   </si>
@@ -117,15 +117,9 @@
     <t>parameters</t>
   </si>
   <si>
-    <t>Down light</t>
-  </si>
-  <si>
     <t>pin action</t>
   </si>
   <si>
-    <t>Down sound</t>
-  </si>
-  <si>
     <t>FLASH</t>
   </si>
   <si>
@@ -172,13 +166,49 @@
   </si>
   <si>
     <t>TONE</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Down light A0</t>
+  </si>
+  <si>
+    <t>Down sound A1</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>C6,1000,PAUSE,500,D6,1000</t>
+  </si>
+  <si>
+    <t>Ignore A2 Inputs</t>
+  </si>
+  <si>
+    <t>Ignore A3 Inputs</t>
+  </si>
+  <si>
+    <t>Ignore A4 Inputs</t>
+  </si>
+  <si>
+    <t>Ignore A5 Inputs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +220,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -218,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -236,6 +272,9 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -551,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{593FC154-758F-4104-A30E-11A530E91792}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -564,7 +603,7 @@
     <col min="3" max="3" width="24.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="9" style="2" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" style="4" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" style="4" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" style="2" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="2"/>
@@ -584,7 +623,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>26</v>
@@ -607,16 +646,16 @@
         <v>13</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -627,16 +666,16 @@
         <v>13</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -647,7 +686,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>5</v>
@@ -661,7 +700,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>4</v>
@@ -678,7 +717,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -690,7 +729,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" ht="30">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -698,13 +737,16 @@
         <v>12</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -712,13 +754,13 @@
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>11</v>
@@ -729,13 +771,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>13</v>
@@ -749,16 +791,16 @@
         <v>9</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" s="3">
         <v>2</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="3"/>
@@ -772,16 +814,16 @@
         <v>9</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11" s="3">
         <v>2</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="3"/>
@@ -795,7 +837,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="9" t="s">
@@ -814,7 +856,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="9" t="s">
@@ -835,7 +877,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D14" s="3">
         <v>2</v>
@@ -858,16 +900,16 @@
         <v>8</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D15" s="3">
         <v>2</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="3"/>
@@ -884,13 +926,13 @@
       <c r="D16" s="3"/>
       <c r="E16" s="9"/>
       <c r="F16" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>18</v>
@@ -911,7 +953,7 @@
         <v>4</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>19</v>
@@ -925,16 +967,16 @@
         <v>5</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D18" s="2">
         <v>3</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -945,16 +987,16 @@
         <v>5</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -965,7 +1007,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>5</v>
@@ -979,7 +1021,7 @@
         <v>5</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>4</v>
@@ -996,7 +1038,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D22" s="2">
         <v>3</v>
@@ -1013,19 +1055,19 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D23" s="2">
         <v>3</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1039,7 +1081,7 @@
         <v>4</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>23</v>
@@ -1056,7 +1098,7 @@
         <v>4</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>25</v>
@@ -1064,13 +1106,13 @@
     </row>
     <row r="26" spans="1:9" s="1" customFormat="1">
       <c r="A26" s="3" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="9" t="s">
@@ -1085,13 +1127,13 @@
     </row>
     <row r="27" spans="1:9" s="1" customFormat="1">
       <c r="A27" s="3" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="9" t="s">
@@ -1104,7 +1146,52 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>